<commit_message>
updated the adder class
</commit_message>
<xml_diff>
--- a/Sample_Company_Data.xlsx
+++ b/Sample_Company_Data.xlsx
@@ -527,7 +527,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -659,14 +658,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="SimSun" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Times New Roman" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme>
@@ -674,58 +673,25 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
+          <a:miter/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:prstDash val="solid"/>
+          <a:miter/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -743,48 +709,12 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
-        <a:gradFill>
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
-        </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -799,7 +729,7 @@
   <dimension ref="A1:B1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:B7"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -808,7 +738,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -816,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -824,7 +754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -832,7 +762,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -840,7 +770,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -848,20 +778,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -884,7 +814,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="1" sqref="A7:B7 D19"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -893,7 +823,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="2" style="1" width="11.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -904,7 +834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -915,7 +845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -926,266 +856,266 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
     </row>
-    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="3"/>
     </row>
-    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="3"/>
     </row>
-    <row r="35" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="3"/>
     </row>
-    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="3"/>
     </row>
-    <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
     </row>
-    <row r="39" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
     </row>
-    <row r="40" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
     </row>
-    <row r="44" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
     </row>
-    <row r="45" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
     </row>
-    <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2"/>
       <c r="C55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2"/>
       <c r="B56" s="2"/>
       <c r="C56" s="3"/>
@@ -1209,7 +1139,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="A7:B7 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1217,7 +1147,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="11.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -1231,7 +1161,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -1245,7 +1175,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1259,7 +1189,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1273,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +1217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>14</v>
       </c>
@@ -1301,7 +1231,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -1315,7 +1245,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1329,7 +1259,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
@@ -1343,7 +1273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -1357,7 +1287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
@@ -1371,7 +1301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>27</v>
       </c>
@@ -1385,7 +1315,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>38</v>
       </c>
@@ -1399,7 +1329,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>38</v>
       </c>
@@ -1413,7 +1343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>38</v>
       </c>
@@ -1427,7 +1357,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
         <v>38</v>
       </c>
@@ -1441,7 +1371,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>47</v>
       </c>
@@ -1455,7 +1385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
         <v>47</v>
       </c>
@@ -1469,7 +1399,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
         <v>47</v>
       </c>
@@ -1483,7 +1413,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
         <v>47</v>
       </c>
@@ -1497,7 +1427,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
         <v>47</v>
       </c>
@@ -1511,7 +1441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
         <v>47</v>
       </c>
@@ -1525,7 +1455,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
         <v>47</v>
       </c>
@@ -1539,7 +1469,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -1553,7 +1483,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>47</v>
       </c>
@@ -1567,7 +1497,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -1581,7 +1511,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>47</v>
       </c>
@@ -1595,7 +1525,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>47</v>
       </c>
@@ -1609,7 +1539,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>47</v>
       </c>
@@ -1623,7 +1553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>47</v>
       </c>
@@ -1637,7 +1567,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>47</v>
       </c>
@@ -1651,7 +1581,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>47</v>
       </c>
@@ -1665,7 +1595,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>47</v>
       </c>
@@ -1679,7 +1609,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>47</v>
       </c>
@@ -1693,7 +1623,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
@@ -1707,7 +1637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
         <v>47</v>
       </c>
@@ -1721,7 +1651,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
         <v>47</v>
       </c>
@@ -1735,7 +1665,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
         <v>47</v>
       </c>
@@ -1749,7 +1679,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="s">
         <v>47</v>
       </c>
@@ -1763,7 +1693,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>47</v>
       </c>
@@ -1777,7 +1707,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
         <v>47</v>
       </c>
@@ -1791,7 +1721,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
         <v>47</v>
       </c>
@@ -1805,7 +1735,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
@@ -1819,7 +1749,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
@@ -1833,7 +1763,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="2" t="s">
         <v>104</v>
       </c>
@@ -1847,7 +1777,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="2" t="s">
         <v>104</v>
       </c>
@@ -1861,7 +1791,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="s">
         <v>104</v>
       </c>
@@ -1875,7 +1805,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="2" t="s">
         <v>104</v>
       </c>
@@ -1889,7 +1819,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="2" t="s">
         <v>104</v>
       </c>
@@ -1903,7 +1833,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="2" t="s">
         <v>104</v>
       </c>
@@ -1917,7 +1847,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="2" t="s">
         <v>104</v>
       </c>
@@ -1931,7 +1861,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="2" t="s">
         <v>104</v>
       </c>
@@ -1945,7 +1875,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
@@ -1959,7 +1889,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
         <v>104</v>
       </c>
@@ -1973,7 +1903,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -1987,7 +1917,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -2001,7 +1931,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -2015,7 +1945,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="s">
         <v>132</v>
       </c>
@@ -2029,7 +1959,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="2" t="s">
         <v>132</v>
       </c>
@@ -2043,7 +1973,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>137</v>
       </c>
@@ -2057,7 +1987,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="s">
         <v>137</v>
       </c>
@@ -2071,7 +2001,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="s">
         <v>137</v>
       </c>
@@ -2085,7 +2015,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="s">
         <v>137</v>
       </c>
@@ -2099,7 +2029,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="s">
         <v>137</v>
       </c>
@@ -2113,7 +2043,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="2" t="s">
         <v>137</v>
       </c>
@@ -2146,7 +2076,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A7:B7 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2155,7 +2085,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2163,7 +2093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>150</v>
       </c>
@@ -2171,7 +2101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>151</v>
       </c>
@@ -2179,7 +2109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>152</v>
       </c>
@@ -2187,7 +2117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>153</v>
       </c>
@@ -2214,7 +2144,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="A7:B7 C4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.45" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2225,7 +2155,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.29"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2239,7 +2169,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>155</v>
       </c>
@@ -2253,7 +2183,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>157</v>
       </c>
@@ -2267,7 +2197,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>158</v>
       </c>
@@ -2281,7 +2211,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>159</v>
       </c>
@@ -2295,7 +2225,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>161</v>
       </c>

</xml_diff>